<commit_message>
Added popular search function to search_twitter_query
</commit_message>
<xml_diff>
--- a/Training Dataset.xlsx
+++ b/Training Dataset.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6440" yWindow="3720" windowWidth="14400" windowHeight="9660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>@microsoft</t>
+  </si>
+  <si>
+    <t>@google</t>
+  </si>
+  <si>
+    <t>@intel</t>
+  </si>
+  <si>
+    <t>@xerox</t>
   </si>
 </sst>
 </file>
@@ -7579,10 +7588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7621,194 +7630,194 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4">
         <v>43051</v>
       </c>
       <c r="C2">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="D2">
-        <v>0.24434638593729499</v>
+        <v>0.146969417318254</v>
       </c>
       <c r="E2">
-        <v>0.137350903515676</v>
+        <v>6.8269488909023804E-2</v>
       </c>
       <c r="F2" s="5">
-        <v>43051.737256944441</v>
+        <v>43051.686574074076</v>
       </c>
       <c r="G2">
-        <v>1851</v>
+        <v>28625</v>
       </c>
       <c r="H2">
-        <v>3195</v>
+        <v>53153</v>
       </c>
       <c r="I2">
-        <v>233135</v>
+        <v>1126288</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4">
         <v>43050</v>
       </c>
       <c r="C3">
-        <v>116</v>
+        <v>279</v>
       </c>
       <c r="D3">
-        <v>0.30329081040287897</v>
+        <v>8.2557513175792699E-2</v>
       </c>
       <c r="E3">
-        <v>-1.28782436433298E-2</v>
+        <v>3.3364406029056499E-2</v>
       </c>
       <c r="F3" s="5">
-        <v>43050.766134259262</v>
+        <v>43050.74318287037</v>
       </c>
       <c r="G3">
-        <v>3602</v>
+        <v>79235</v>
       </c>
       <c r="H3">
-        <v>5794</v>
+        <v>147363</v>
       </c>
       <c r="I3">
-        <v>2979831</v>
+        <v>1164567</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4">
         <v>43049</v>
       </c>
       <c r="C4">
-        <v>317</v>
+        <v>176</v>
       </c>
       <c r="D4">
-        <v>0.30152832971444898</v>
+        <v>0.27184386478420502</v>
       </c>
       <c r="E4">
-        <v>2.4389671842353199E-2</v>
+        <v>0.141242662009707</v>
       </c>
       <c r="F4" s="5">
-        <v>43049.743958333333</v>
+        <v>43049.708437499998</v>
       </c>
       <c r="G4">
-        <v>5016</v>
+        <v>2328</v>
       </c>
       <c r="H4">
-        <v>5528</v>
+        <v>4873</v>
       </c>
       <c r="I4">
-        <v>4077264</v>
+        <v>903368</v>
       </c>
       <c r="J4">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4">
         <v>43051</v>
       </c>
       <c r="C5">
-        <v>129</v>
+        <v>436</v>
       </c>
       <c r="D5">
-        <v>0.146969417318254</v>
+        <v>0.343027030627374</v>
       </c>
       <c r="E5">
-        <v>6.8269488909023804E-2</v>
+        <v>0.126860207994095</v>
       </c>
       <c r="F5" s="5">
-        <v>43051.686574074076</v>
+        <v>43051.734050925923</v>
       </c>
       <c r="G5">
-        <v>28625</v>
+        <v>18030</v>
       </c>
       <c r="H5">
-        <v>53153</v>
+        <v>47139</v>
       </c>
       <c r="I5">
-        <v>1126288</v>
+        <v>2382266</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4">
         <v>43050</v>
       </c>
       <c r="C6">
-        <v>279</v>
+        <v>589</v>
       </c>
       <c r="D6">
-        <v>8.2557513175792699E-2</v>
+        <v>0.35341159901219299</v>
       </c>
       <c r="E6">
-        <v>3.3364406029056499E-2</v>
+        <v>0.16138898961303799</v>
       </c>
       <c r="F6" s="5">
-        <v>43050.74318287037</v>
+        <v>43050.707754629628</v>
       </c>
       <c r="G6">
-        <v>79235</v>
+        <v>26334</v>
       </c>
       <c r="H6">
-        <v>147363</v>
+        <v>91877</v>
       </c>
       <c r="I6">
-        <v>1164567</v>
+        <v>2926112</v>
       </c>
       <c r="J6">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4">
         <v>43049</v>
       </c>
       <c r="C7">
-        <v>176</v>
+        <v>1067</v>
       </c>
       <c r="D7">
-        <v>0.27184386478420502</v>
+        <v>0.31842923759394998</v>
       </c>
       <c r="E7">
-        <v>0.141242662009707</v>
+        <v>0.123030835252601</v>
       </c>
       <c r="F7" s="5">
-        <v>43049.708437499998</v>
+        <v>43049.725185185183</v>
       </c>
       <c r="G7">
-        <v>2328</v>
+        <v>54681</v>
       </c>
       <c r="H7">
-        <v>4873</v>
+        <v>159766</v>
       </c>
       <c r="I7">
-        <v>903368</v>
+        <v>16890622</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -7816,31 +7825,31 @@
         <v>33</v>
       </c>
       <c r="B8" s="4">
-        <v>43051</v>
+        <v>43048</v>
       </c>
       <c r="C8">
-        <v>436</v>
+        <v>1350</v>
       </c>
       <c r="D8">
-        <v>0.343027030627374</v>
+        <v>0.34686815821352801</v>
       </c>
       <c r="E8">
-        <v>0.126860207994095</v>
+        <v>0.12900209803057</v>
       </c>
       <c r="F8" s="5">
-        <v>43051.734050925923</v>
+        <v>43048.738518518519</v>
       </c>
       <c r="G8">
-        <v>18030</v>
+        <v>132180</v>
       </c>
       <c r="H8">
-        <v>47139</v>
+        <v>472977</v>
       </c>
       <c r="I8">
-        <v>2382266</v>
+        <v>12224187</v>
       </c>
       <c r="J8">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -7848,31 +7857,31 @@
         <v>33</v>
       </c>
       <c r="B9" s="4">
-        <v>43050</v>
+        <v>43047</v>
       </c>
       <c r="C9">
-        <v>589</v>
+        <v>2589</v>
       </c>
       <c r="D9">
-        <v>0.35341159901219299</v>
+        <v>0.296453870096689</v>
       </c>
       <c r="E9">
-        <v>0.16138898961303799</v>
+        <v>0.13364892356750899</v>
       </c>
       <c r="F9" s="5">
-        <v>43050.707754629628</v>
+        <v>43047.727800925924</v>
       </c>
       <c r="G9">
-        <v>26334</v>
+        <v>886006</v>
       </c>
       <c r="H9">
-        <v>91877</v>
+        <v>5678150</v>
       </c>
       <c r="I9">
-        <v>2926112</v>
+        <v>10942134</v>
       </c>
       <c r="J9">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -7880,31 +7889,31 @@
         <v>33</v>
       </c>
       <c r="B10" s="4">
-        <v>43049</v>
+        <v>43046</v>
       </c>
       <c r="C10">
-        <v>1067</v>
+        <v>1884</v>
       </c>
       <c r="D10">
-        <v>0.31842923759394998</v>
+        <v>0.33530867000519299</v>
       </c>
       <c r="E10">
-        <v>0.123030835252601</v>
+        <v>0.120278928433129</v>
       </c>
       <c r="F10" s="5">
-        <v>43049.725185185183</v>
+        <v>43046.738009259258</v>
       </c>
       <c r="G10">
-        <v>54681</v>
+        <v>67370</v>
       </c>
       <c r="H10">
-        <v>159766</v>
+        <v>455760</v>
       </c>
       <c r="I10">
-        <v>16890622</v>
+        <v>15655615</v>
       </c>
       <c r="J10">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -7912,127 +7921,895 @@
         <v>33</v>
       </c>
       <c r="B11" s="4">
-        <v>43048</v>
+        <v>43045</v>
       </c>
       <c r="C11">
-        <v>1350</v>
+        <v>1246</v>
       </c>
       <c r="D11">
-        <v>0.34686815821352801</v>
+        <v>0.33793314571404398</v>
       </c>
       <c r="E11">
-        <v>0.12900209803057</v>
+        <v>0.142007954323112</v>
       </c>
       <c r="F11" s="5">
-        <v>43048.738518518519</v>
+        <v>43045.759756944448</v>
       </c>
       <c r="G11">
-        <v>132180</v>
+        <v>55237</v>
       </c>
       <c r="H11">
-        <v>472977</v>
+        <v>305135</v>
       </c>
       <c r="I11">
-        <v>12224187</v>
+        <v>24069567</v>
       </c>
       <c r="J11">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4">
-        <v>43047</v>
+        <v>43051</v>
       </c>
       <c r="C12">
-        <v>2589</v>
+        <v>1154</v>
       </c>
       <c r="D12">
-        <v>0.296453870096689</v>
+        <v>0.26658532433770699</v>
       </c>
       <c r="E12">
-        <v>0.13364892356750899</v>
+        <v>8.9615147644014501E-2</v>
       </c>
       <c r="F12" s="5">
-        <v>43047.727800925924</v>
+        <v>43051.73269675926</v>
       </c>
       <c r="G12">
-        <v>886006</v>
+        <v>621286</v>
       </c>
       <c r="H12">
-        <v>5678150</v>
+        <v>1879527</v>
       </c>
       <c r="I12">
-        <v>10942134</v>
+        <v>5276634</v>
       </c>
       <c r="J12">
-        <v>69</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="4">
-        <v>43046</v>
+        <v>43050</v>
       </c>
       <c r="C13">
-        <v>1884</v>
+        <v>1741</v>
       </c>
       <c r="D13">
-        <v>0.33530867000519299</v>
+        <v>0.29256185580539301</v>
       </c>
       <c r="E13">
-        <v>0.120278928433129</v>
+        <v>0.14962077861037701</v>
       </c>
       <c r="F13" s="5">
-        <v>43046.738009259258</v>
+        <v>43050.733900462961</v>
       </c>
       <c r="G13">
-        <v>67370</v>
+        <v>634177</v>
       </c>
       <c r="H13">
-        <v>455760</v>
+        <v>1717773</v>
       </c>
       <c r="I13">
-        <v>15655615</v>
+        <v>18651373</v>
       </c>
       <c r="J13">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="4">
+        <v>43049</v>
+      </c>
+      <c r="C14">
+        <v>2410</v>
+      </c>
+      <c r="D14">
+        <v>0.32025905675697902</v>
+      </c>
+      <c r="E14">
+        <v>0.20481043345233901</v>
+      </c>
+      <c r="F14" s="5">
+        <v>43049.70853009259</v>
+      </c>
+      <c r="G14">
+        <v>728970</v>
+      </c>
+      <c r="H14">
+        <v>1882366</v>
+      </c>
+      <c r="I14">
+        <v>14133192</v>
+      </c>
+      <c r="J14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43048</v>
+      </c>
+      <c r="C15">
+        <v>2731</v>
+      </c>
+      <c r="D15">
+        <v>0.27931995132699999</v>
+      </c>
+      <c r="E15">
+        <v>0.11826768599297099</v>
+      </c>
+      <c r="F15" s="5">
+        <v>43048.746863425928</v>
+      </c>
+      <c r="G15">
+        <v>528803</v>
+      </c>
+      <c r="H15">
+        <v>1260719</v>
+      </c>
+      <c r="I15">
+        <v>22383865</v>
+      </c>
+      <c r="J15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4">
+        <v>43047</v>
+      </c>
+      <c r="C16">
+        <v>2420</v>
+      </c>
+      <c r="D16">
+        <v>0.35751104466393502</v>
+      </c>
+      <c r="E16">
+        <v>0.190866551140214</v>
+      </c>
+      <c r="F16" s="5">
+        <v>43047.742604166669</v>
+      </c>
+      <c r="G16">
+        <v>741334</v>
+      </c>
+      <c r="H16">
+        <v>1855603</v>
+      </c>
+      <c r="I16">
+        <v>17160497</v>
+      </c>
+      <c r="J16">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4">
+        <v>43046</v>
+      </c>
+      <c r="C17">
+        <v>2662</v>
+      </c>
+      <c r="D17">
+        <v>0.36730168595213902</v>
+      </c>
+      <c r="E17">
+        <v>0.181640862778576</v>
+      </c>
+      <c r="F17" s="5">
+        <v>43046.752627314818</v>
+      </c>
+      <c r="G17">
+        <v>889832</v>
+      </c>
+      <c r="H17">
+        <v>2736449</v>
+      </c>
+      <c r="I17">
+        <v>34626861</v>
+      </c>
+      <c r="J17">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4">
         <v>43045</v>
       </c>
-      <c r="C14">
-        <v>1246</v>
-      </c>
-      <c r="D14">
-        <v>0.33793314571404398</v>
-      </c>
-      <c r="E14">
-        <v>0.142007954323112</v>
-      </c>
-      <c r="F14" s="5">
-        <v>43045.759756944448</v>
-      </c>
-      <c r="G14">
-        <v>55237</v>
-      </c>
-      <c r="H14">
-        <v>305135</v>
-      </c>
-      <c r="I14">
-        <v>24069567</v>
-      </c>
-      <c r="J14">
-        <v>81</v>
+      <c r="C18">
+        <v>3190</v>
+      </c>
+      <c r="D18">
+        <v>0.42111298215020498</v>
+      </c>
+      <c r="E18">
+        <v>0.17602118392934399</v>
+      </c>
+      <c r="F18" s="5">
+        <v>43045.75341435185</v>
+      </c>
+      <c r="G18">
+        <v>1322624</v>
+      </c>
+      <c r="H18">
+        <v>3717511</v>
+      </c>
+      <c r="I18">
+        <v>15641992</v>
+      </c>
+      <c r="J18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43051</v>
+      </c>
+      <c r="C19">
+        <v>159</v>
+      </c>
+      <c r="D19">
+        <v>0.21754086235218301</v>
+      </c>
+      <c r="E19">
+        <v>8.9408282907693301E-2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>43051.742650462962</v>
+      </c>
+      <c r="G19">
+        <v>16500</v>
+      </c>
+      <c r="H19">
+        <v>68519</v>
+      </c>
+      <c r="I19">
+        <v>913879</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43050</v>
+      </c>
+      <c r="C20">
+        <v>224</v>
+      </c>
+      <c r="D20">
+        <v>0.28473008142650902</v>
+      </c>
+      <c r="E20">
+        <v>0.102158426580859</v>
+      </c>
+      <c r="F20" s="5">
+        <v>43050.723182870373</v>
+      </c>
+      <c r="G20">
+        <v>13316</v>
+      </c>
+      <c r="H20">
+        <v>61867</v>
+      </c>
+      <c r="I20">
+        <v>1100498</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="4">
+        <v>43049</v>
+      </c>
+      <c r="C21">
+        <v>330</v>
+      </c>
+      <c r="D21">
+        <v>0.31613144066931897</v>
+      </c>
+      <c r="E21">
+        <v>0.153106849519728</v>
+      </c>
+      <c r="F21" s="5">
+        <v>43049.739583333336</v>
+      </c>
+      <c r="G21">
+        <v>19854</v>
+      </c>
+      <c r="H21">
+        <v>73869</v>
+      </c>
+      <c r="I21">
+        <v>4077966</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4">
+        <v>43048</v>
+      </c>
+      <c r="C22">
+        <v>459</v>
+      </c>
+      <c r="D22">
+        <v>0.4009750778351</v>
+      </c>
+      <c r="E22">
+        <v>0.16450478203814201</v>
+      </c>
+      <c r="F22" s="5">
+        <v>43048.753703703704</v>
+      </c>
+      <c r="G22">
+        <v>33208</v>
+      </c>
+      <c r="H22">
+        <v>125272</v>
+      </c>
+      <c r="I22">
+        <v>11336102</v>
+      </c>
+      <c r="J22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4">
+        <v>43047</v>
+      </c>
+      <c r="C23">
+        <v>504</v>
+      </c>
+      <c r="D23">
+        <v>0.474238594848714</v>
+      </c>
+      <c r="E23">
+        <v>0.24211280892828399</v>
+      </c>
+      <c r="F23" s="5">
+        <v>43047.760081018518</v>
+      </c>
+      <c r="G23">
+        <v>61916</v>
+      </c>
+      <c r="H23">
+        <v>90765</v>
+      </c>
+      <c r="I23">
+        <v>10820240</v>
+      </c>
+      <c r="J23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4">
+        <v>43046</v>
+      </c>
+      <c r="C24">
+        <v>937</v>
+      </c>
+      <c r="D24">
+        <v>0.48897134941425102</v>
+      </c>
+      <c r="E24">
+        <v>0.33080688151526</v>
+      </c>
+      <c r="F24" s="5">
+        <v>43046.781273148146</v>
+      </c>
+      <c r="G24">
+        <v>178084</v>
+      </c>
+      <c r="H24">
+        <v>285854</v>
+      </c>
+      <c r="I24">
+        <v>9479257</v>
+      </c>
+      <c r="J24">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43045</v>
+      </c>
+      <c r="C25">
+        <v>484</v>
+      </c>
+      <c r="D25">
+        <v>0.29815142893913499</v>
+      </c>
+      <c r="E25">
+        <v>0.13110979131402101</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43045.750960648147</v>
+      </c>
+      <c r="G25">
+        <v>29272</v>
+      </c>
+      <c r="H25">
+        <v>146553</v>
+      </c>
+      <c r="I25">
+        <v>5138084</v>
+      </c>
+      <c r="J25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="4">
+        <v>43051</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0.27913299663299601</v>
+      </c>
+      <c r="E26">
+        <v>2.5101010101009999E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>43051.687407407408</v>
+      </c>
+      <c r="G26">
+        <v>318</v>
+      </c>
+      <c r="H26">
+        <v>724</v>
+      </c>
+      <c r="I26">
+        <v>511258</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4">
+        <v>43050</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>0.25883065347350998</v>
+      </c>
+      <c r="E27">
+        <v>8.5006527863670703E-2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>43050.724143518521</v>
+      </c>
+      <c r="G27">
+        <v>420</v>
+      </c>
+      <c r="H27">
+        <v>862</v>
+      </c>
+      <c r="I27">
+        <v>54216</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43049</v>
+      </c>
+      <c r="C28">
+        <v>72</v>
+      </c>
+      <c r="D28">
+        <v>0.27216435185185101</v>
+      </c>
+      <c r="E28">
+        <v>0.106828703703703</v>
+      </c>
+      <c r="F28" s="5">
+        <v>43049.750486111108</v>
+      </c>
+      <c r="G28">
+        <v>540</v>
+      </c>
+      <c r="H28">
+        <v>1323</v>
+      </c>
+      <c r="I28">
+        <v>3708280</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43048</v>
+      </c>
+      <c r="C29">
+        <v>67</v>
+      </c>
+      <c r="D29">
+        <v>0.33552691090004499</v>
+      </c>
+      <c r="E29">
+        <v>0.12507538067239499</v>
+      </c>
+      <c r="F29" s="5">
+        <v>43048.77888888889</v>
+      </c>
+      <c r="G29">
+        <v>482</v>
+      </c>
+      <c r="H29">
+        <v>559</v>
+      </c>
+      <c r="I29">
+        <v>577345</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="4">
+        <v>43047</v>
+      </c>
+      <c r="C30">
+        <v>64</v>
+      </c>
+      <c r="D30">
+        <v>0.274767203282828</v>
+      </c>
+      <c r="E30">
+        <v>0.18637547348484801</v>
+      </c>
+      <c r="F30" s="5">
+        <v>43047.777916666666</v>
+      </c>
+      <c r="G30">
+        <v>504</v>
+      </c>
+      <c r="H30">
+        <v>320</v>
+      </c>
+      <c r="I30">
+        <v>55167</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="4">
+        <v>43046</v>
+      </c>
+      <c r="C31">
+        <v>76</v>
+      </c>
+      <c r="D31">
+        <v>0.33938230994152002</v>
+      </c>
+      <c r="E31">
+        <v>0.26217105263157803</v>
+      </c>
+      <c r="F31" s="5">
+        <v>43046.809328703705</v>
+      </c>
+      <c r="G31">
+        <v>860</v>
+      </c>
+      <c r="H31">
+        <v>587</v>
+      </c>
+      <c r="I31">
+        <v>56512</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="4">
+        <v>43045</v>
+      </c>
+      <c r="C32">
+        <v>42</v>
+      </c>
+      <c r="D32">
+        <v>0.18249458874458799</v>
+      </c>
+      <c r="E32">
+        <v>0.10340909090909001</v>
+      </c>
+      <c r="F32" s="5">
+        <v>43045.735092592593</v>
+      </c>
+      <c r="G32">
+        <v>398</v>
+      </c>
+      <c r="H32">
+        <v>598</v>
+      </c>
+      <c r="I32">
+        <v>195108</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <v>43051</v>
+      </c>
+      <c r="C33">
+        <v>112</v>
+      </c>
+      <c r="D33">
+        <v>0.23998305761698599</v>
+      </c>
+      <c r="E33">
+        <v>0.134898208810039</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43051.739814814813</v>
+      </c>
+      <c r="G33">
+        <v>2032</v>
+      </c>
+      <c r="H33">
+        <v>3489</v>
+      </c>
+      <c r="I33">
+        <v>233753</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4">
+        <v>43050</v>
+      </c>
+      <c r="C34">
+        <v>114</v>
+      </c>
+      <c r="D34">
+        <v>0.30412827101423501</v>
+      </c>
+      <c r="E34">
+        <v>-1.43225013290802E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>43050.766134259262</v>
+      </c>
+      <c r="G34">
+        <v>3622</v>
+      </c>
+      <c r="H34">
+        <v>5838</v>
+      </c>
+      <c r="I34">
+        <v>2978744</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="4">
+        <v>43049</v>
+      </c>
+      <c r="C35">
+        <v>318</v>
+      </c>
+      <c r="D35">
+        <v>0.30267656347845001</v>
+      </c>
+      <c r="E35">
+        <v>2.21117168994527E-2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>43049.743958333333</v>
+      </c>
+      <c r="G35">
+        <v>5095</v>
+      </c>
+      <c r="H35">
+        <v>5580</v>
+      </c>
+      <c r="I35">
+        <v>4078743</v>
+      </c>
+      <c r="J35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4">
+        <v>43048</v>
+      </c>
+      <c r="C36">
+        <v>295</v>
+      </c>
+      <c r="D36">
+        <v>0.33827825470198303</v>
+      </c>
+      <c r="E36">
+        <v>0.20487648924169</v>
+      </c>
+      <c r="F36" s="5">
+        <v>43048.718877314815</v>
+      </c>
+      <c r="G36">
+        <v>1423</v>
+      </c>
+      <c r="H36">
+        <v>4078</v>
+      </c>
+      <c r="I36">
+        <v>1407384</v>
+      </c>
+      <c r="J36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="4">
+        <v>43047</v>
+      </c>
+      <c r="C37">
+        <v>365</v>
+      </c>
+      <c r="D37">
+        <v>0.29435063946707801</v>
+      </c>
+      <c r="E37">
+        <v>0.14133754950022001</v>
+      </c>
+      <c r="F37" s="5">
+        <v>43047.739583333336</v>
+      </c>
+      <c r="G37">
+        <v>3305</v>
+      </c>
+      <c r="H37">
+        <v>7341</v>
+      </c>
+      <c r="I37">
+        <v>1959983</v>
+      </c>
+      <c r="J37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="4">
+        <v>43046</v>
+      </c>
+      <c r="C38">
+        <v>464</v>
+      </c>
+      <c r="D38">
+        <v>0.25981911557073101</v>
+      </c>
+      <c r="E38">
+        <v>0.15519593448338001</v>
+      </c>
+      <c r="F38" s="5">
+        <v>43046.74119212963</v>
+      </c>
+      <c r="G38">
+        <v>4224</v>
+      </c>
+      <c r="H38">
+        <v>5594</v>
+      </c>
+      <c r="I38">
+        <v>1855143</v>
+      </c>
+      <c r="J38">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>